<commit_message>
monday entry + raw combination srb data
</commit_message>
<xml_diff>
--- a/Protocols/Drug_combination_concentrations.xlsx
+++ b/Protocols/Drug_combination_concentrations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyal Dass\Documents\SRB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyal Dass\Documents\GitHub\PD_Lab_book\Protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Crizotinib</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Final conc</t>
   </si>
   <si>
-    <t>11x conc</t>
-  </si>
-  <si>
     <t>Final conc (uM)</t>
   </si>
   <si>
@@ -84,6 +81,18 @@
   </si>
   <si>
     <t>S volume</t>
+  </si>
+  <si>
+    <t>Add 97.19uL SFM</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Add 95.77uL SFM</t>
+  </si>
+  <si>
+    <t>Add 96.90uL SFM</t>
   </si>
 </sst>
 </file>
@@ -204,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,6 +270,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -550,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +626,9 @@
         <v>0</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -632,7 +646,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>2</v>
@@ -644,7 +658,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -656,10 +670,10 @@
         <v>0</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="17">
         <v>3.1019999999999999</v>
@@ -822,7 +836,9 @@
         <v>1</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -840,7 +856,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>2</v>
@@ -864,10 +880,10 @@
         <v>0</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22" s="17">
         <v>2.8125624999999999</v>
@@ -897,7 +913,7 @@
         <v>1.6875374999999997</v>
       </c>
       <c r="G23" s="17">
-        <f t="shared" ref="G23:G28" si="5">4.091*B23</f>
+        <f>4.091*B23</f>
         <v>0.40910000000000002</v>
       </c>
     </row>
@@ -913,15 +929,15 @@
         <v>0.4</v>
       </c>
       <c r="E24" s="17">
-        <f t="shared" ref="E24:E28" si="6">G24/D24*1.1</f>
+        <f t="shared" ref="E24:E28" si="5">G24/D24*1.1</f>
         <v>2.8125624999999999</v>
       </c>
       <c r="F24" s="17">
-        <f t="shared" ref="F24:F28" si="7">2.8125625-E24</f>
+        <f t="shared" ref="F24:F28" si="6">2.8125625-E24</f>
         <v>0</v>
       </c>
       <c r="G24" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="G23:G28" si="7">4.091*B24</f>
         <v>1.02275</v>
       </c>
     </row>
@@ -937,15 +953,15 @@
         <v>4</v>
       </c>
       <c r="E25" s="17">
+        <f t="shared" si="5"/>
+        <v>0.56251250000000008</v>
+      </c>
+      <c r="F25" s="17">
         <f t="shared" si="6"/>
-        <v>0.56251250000000008</v>
-      </c>
-      <c r="F25" s="17">
+        <v>2.2500499999999999</v>
+      </c>
+      <c r="G25" s="17">
         <f t="shared" si="7"/>
-        <v>2.2500499999999999</v>
-      </c>
-      <c r="G25" s="17">
-        <f t="shared" si="5"/>
         <v>2.0455000000000001</v>
       </c>
     </row>
@@ -961,15 +977,15 @@
         <v>4</v>
       </c>
       <c r="E26" s="17">
+        <f t="shared" si="5"/>
+        <v>1.1250250000000002</v>
+      </c>
+      <c r="F26" s="17">
         <f t="shared" si="6"/>
-        <v>1.1250250000000002</v>
-      </c>
-      <c r="F26" s="17">
+        <v>1.6875374999999997</v>
+      </c>
+      <c r="G26" s="17">
         <f t="shared" si="7"/>
-        <v>1.6875374999999997</v>
-      </c>
-      <c r="G26" s="17">
-        <f t="shared" si="5"/>
         <v>4.0910000000000002</v>
       </c>
     </row>
@@ -985,15 +1001,15 @@
         <v>40</v>
       </c>
       <c r="E27" s="17">
+        <f t="shared" si="5"/>
+        <v>0.28125625000000004</v>
+      </c>
+      <c r="F27" s="17">
         <f t="shared" si="6"/>
-        <v>0.28125625000000004</v>
-      </c>
-      <c r="F27" s="17">
+        <v>2.5313062499999996</v>
+      </c>
+      <c r="G27" s="17">
         <f t="shared" si="7"/>
-        <v>2.5313062499999996</v>
-      </c>
-      <c r="G27" s="17">
-        <f t="shared" si="5"/>
         <v>10.227500000000001</v>
       </c>
     </row>
@@ -1009,21 +1025,24 @@
         <v>40</v>
       </c>
       <c r="E28" s="17">
+        <f t="shared" si="5"/>
+        <v>0.56251250000000008</v>
+      </c>
+      <c r="F28" s="17">
         <f t="shared" si="6"/>
-        <v>0.56251250000000008</v>
-      </c>
-      <c r="F28" s="17">
+        <v>2.2500499999999999</v>
+      </c>
+      <c r="G28" s="17">
         <f t="shared" si="7"/>
-        <v>2.2500499999999999</v>
-      </c>
-      <c r="G28" s="17">
-        <f t="shared" si="5"/>
         <v>20.455000000000002</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -1031,16 +1050,16 @@
         <v>9</v>
       </c>
       <c r="C38" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="E38" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="F38" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>19</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>3</v>
@@ -1051,16 +1070,16 @@
         <v>0</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39" s="17">
         <v>4.2270250000000003</v>

</xml_diff>